<commit_message>
lendo xlsx, mntndo array e obtendo dados   ok
</commit_message>
<xml_diff>
--- a/python/TestesAutomatizados/PDV2/cenariosDeTeste.xlsx
+++ b/python/TestesAutomatizados/PDV2/cenariosDeTeste.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9975" windowHeight="6060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Venda" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Ativo</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Verificar se o sistema não teve alteração na leitura dos produtos</t>
+  </si>
+  <si>
+    <t>Venda de um item com quantidade acima de 1</t>
+  </si>
+  <si>
+    <t>Inserir o código manualmente com quantidade 3</t>
+  </si>
+  <si>
+    <t>Verificar se o sistema não teve impacto ao inserir quantidade superior a 1</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -603,7 +612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -620,39 +629,39 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5">
         <v>1030048</v>
       </c>
       <c r="C4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
@@ -660,10 +669,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="5">
-        <v>1030050</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
+        <v>1030048</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
@@ -678,6 +687,32 @@
         <v>17</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1030050</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
waiting if is kit
</commit_message>
<xml_diff>
--- a/python/TestesAutomatizados/PDV2/cenariosDeTeste.xlsx
+++ b/python/TestesAutomatizados/PDV2/cenariosDeTeste.xlsx
@@ -450,8 +450,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,7 +463,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="23.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="43.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="53.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>